<commit_message>
Actualizado GitIgnore, eliminados ficheros de configuración propios de UiPath, modificado BuscarSolicitud
</commit_message>
<xml_diff>
--- a/ARR_001_001_Certificados/Data/Config.xlsx
+++ b/ARR_001_001_Certificados/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\ARR_001_001_Certificados\ARR_001_001_Certificados\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36D7AD0-CAE1-4627-8754-FD0BFC9CB2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC10098C-D016-45E1-A0AC-A3D431AD41CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="23010" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>